<commit_message>
Modification du tableau des prochains adversaires, pour ne plus avoir de problèmes sur la fin de saison (moins de matchs restants que le nombre d'adversaires demandés)
</commit_message>
<xml_diff>
--- a/Excel/TI/Mon_TI_2024_04_06.xlsx
+++ b/Excel/TI/Mon_TI_2024_04_06.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AL16"/>
+  <dimension ref="A1:AL18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -628,19 +628,15 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>LAL</t>
+          <t>PHI</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Anthony Davis</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Questionable</t>
-        </is>
-      </c>
+          <t>Joel Embiid</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
           <t>C</t>
@@ -648,73 +644,79 @@
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="n">
-        <v>54</v>
+        <v>50.4</v>
       </c>
       <c r="G2" t="n">
-        <v>48.1</v>
+        <v>60.3</v>
       </c>
       <c r="H2" t="n">
-        <v>47.9</v>
+        <v>59.9</v>
       </c>
       <c r="I2" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="J2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
         <v>1</v>
       </c>
       <c r="M2" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="N2" t="n">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="O2" t="n">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P2" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="Q2" t="n">
-        <v>59</v>
-      </c>
-      <c r="R2" t="n">
-        <v>70</v>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="T2" t="n">
-        <v>1</v>
+        <v>-5.2</v>
       </c>
       <c r="U2" t="inlineStr"/>
       <c r="V2" t="inlineStr"/>
       <c r="W2" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="Z2" t="n">
-        <v>59</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="AA2" t="inlineStr">
         <is>
@@ -738,12 +740,12 @@
       </c>
       <c r="AE2" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AF2" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>SAS</t>
         </is>
       </c>
       <c r="AG2" t="inlineStr">
@@ -753,27 +755,27 @@
       </c>
       <c r="AH2" t="inlineStr">
         <is>
-          <t>GSW</t>
+          <t>DET</t>
         </is>
       </c>
       <c r="AI2" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AJ2" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>ORL</t>
         </is>
       </c>
       <c r="AK2" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AL2" t="inlineStr">
         <is>
-          <t>NOP</t>
+          <t>BKN</t>
         </is>
       </c>
     </row>
@@ -788,11 +790,7 @@
           <t>LeBron James</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Questionable</t>
-        </is>
-      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
           <t>F</t>
@@ -800,10 +798,10 @@
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="n">
-        <v>44.4</v>
+        <v>47.2</v>
       </c>
       <c r="G3" t="n">
-        <v>47.1</v>
+        <v>45.9</v>
       </c>
       <c r="H3" t="n">
         <v>42.3</v>
@@ -818,27 +816,25 @@
         <v>1</v>
       </c>
       <c r="L3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N3" t="n">
+        <v>44</v>
+      </c>
+      <c r="O3" t="n">
+        <v>43</v>
+      </c>
+      <c r="P3" t="n">
         <v>69</v>
       </c>
-      <c r="O3" t="n">
+      <c r="Q3" t="n">
         <v>30</v>
       </c>
-      <c r="P3" t="n">
+      <c r="R3" t="n">
         <v>50</v>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R3" t="n">
-        <v>45</v>
       </c>
       <c r="S3" t="inlineStr">
         <is>
@@ -932,12 +928,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>PHI</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Donovan Mitchell</t>
+          <t>Tyrese Maxey</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -948,49 +944,47 @@
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
-        <v>16</v>
+        <v>37.4</v>
       </c>
       <c r="G4" t="n">
-        <v>33.5</v>
+        <v>34.2</v>
       </c>
       <c r="H4" t="n">
-        <v>37.9</v>
+        <v>35.4</v>
       </c>
       <c r="I4" t="n">
+        <v>11</v>
+      </c>
+      <c r="J4" t="n">
+        <v>2</v>
+      </c>
+      <c r="K4" t="n">
+        <v>2</v>
+      </c>
+      <c r="L4" t="n">
+        <v>3</v>
+      </c>
+      <c r="M4" t="n">
         <v>4</v>
       </c>
-      <c r="J4" t="n">
-        <v>4</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0</v>
-      </c>
       <c r="N4" t="n">
-        <v>15</v>
-      </c>
-      <c r="O4" t="n">
-        <v>17</v>
+        <v>60</v>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="Q4" t="n">
+        <v>7</v>
+      </c>
+      <c r="R4" t="n">
+        <v>42</v>
       </c>
       <c r="S4" t="inlineStr">
         <is>
@@ -998,7 +992,7 @@
         </is>
       </c>
       <c r="T4" t="n">
-        <v>-4.3</v>
+        <v>-0.9</v>
       </c>
       <c r="U4" t="inlineStr"/>
       <c r="V4" t="inlineStr"/>
@@ -1009,16 +1003,18 @@
       </c>
       <c r="X4" t="inlineStr">
         <is>
-          <t>LAL</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="Y4" t="inlineStr">
         <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="Z4" t="n">
-        <v>32</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="AA4" t="inlineStr">
         <is>
@@ -1047,7 +1043,7 @@
       </c>
       <c r="AF4" t="inlineStr">
         <is>
-          <t>LAC</t>
+          <t>SAS</t>
         </is>
       </c>
       <c r="AG4" t="inlineStr">
@@ -1057,7 +1053,7 @@
       </c>
       <c r="AH4" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>DET</t>
         </is>
       </c>
       <c r="AI4" t="inlineStr">
@@ -1067,7 +1063,7 @@
       </c>
       <c r="AJ4" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>ORL</t>
         </is>
       </c>
       <c r="AK4" t="inlineStr">
@@ -1077,19 +1073,19 @@
       </c>
       <c r="AL4" t="inlineStr">
         <is>
-          <t>CHA</t>
+          <t>BKN</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>DET</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Cade Cunningham</t>
+          <t>Donovan Mitchell</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
@@ -1098,48 +1094,44 @@
           <t>G</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>O</t>
-        </is>
-      </c>
+      <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
-        <v>39.2</v>
+        <v>18.6</v>
       </c>
       <c r="G5" t="n">
-        <v>33.5</v>
+        <v>33.7</v>
       </c>
       <c r="H5" t="n">
-        <v>32.1</v>
+        <v>37.9</v>
       </c>
       <c r="I5" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="J5" t="n">
+        <v>4</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
         <v>1</v>
       </c>
-      <c r="K5" t="n">
-        <v>4</v>
-      </c>
-      <c r="L5" t="n">
-        <v>3</v>
-      </c>
       <c r="M5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="N5" t="n">
-        <v>59</v>
-      </c>
-      <c r="O5" t="n">
-        <v>44</v>
+        <v>34</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="P5" t="n">
-        <v>38</v>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>15</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>17</v>
       </c>
       <c r="R5" t="inlineStr">
         <is>
@@ -1152,14 +1144,10 @@
         </is>
       </c>
       <c r="T5" t="n">
-        <v>-1.6</v>
-      </c>
-      <c r="U5" t="n">
-        <v>2</v>
-      </c>
-      <c r="V5" t="n">
-        <v>8</v>
-      </c>
+        <v>-4.3</v>
+      </c>
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
       <c r="W5" t="inlineStr">
         <is>
           <t>@</t>
@@ -1167,7 +1155,7 @@
       </c>
       <c r="X5" t="inlineStr">
         <is>
-          <t>BKN</t>
+          <t>LAL</t>
         </is>
       </c>
       <c r="Y5" t="inlineStr">
@@ -1176,23 +1164,27 @@
         </is>
       </c>
       <c r="Z5" t="n">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="AA5" t="inlineStr">
         <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AB5" t="n">
-        <v>71</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="AC5" t="inlineStr">
         <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="AD5" t="n">
-        <v>26</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="AE5" t="inlineStr">
         <is>
@@ -1201,7 +1193,7 @@
       </c>
       <c r="AF5" t="inlineStr">
         <is>
-          <t>PHI</t>
+          <t>LAC</t>
         </is>
       </c>
       <c r="AG5" t="inlineStr">
@@ -1211,92 +1203,86 @@
       </c>
       <c r="AH5" t="inlineStr">
         <is>
-          <t>CHI</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="AI5" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AJ5" t="inlineStr">
         <is>
-          <t>DAL</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="AK5" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AL5" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>CHA</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>PHI</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Tyrese Maxey</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Questionable</t>
-        </is>
-      </c>
+          <t>Evan Mobley</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>C</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="n">
-        <v>31</v>
+        <v>37.8</v>
       </c>
       <c r="G6" t="n">
-        <v>32.5</v>
+        <v>33.1</v>
       </c>
       <c r="H6" t="n">
-        <v>35</v>
+        <v>32.7</v>
       </c>
       <c r="I6" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="J6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K6" t="n">
         <v>2</v>
       </c>
       <c r="L6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M6" t="n">
-        <v>3</v>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>4</v>
+      </c>
+      <c r="N6" t="n">
+        <v>40</v>
       </c>
       <c r="O6" t="n">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="P6" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q6" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="R6" t="n">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="S6" t="inlineStr">
         <is>
@@ -1304,7 +1290,7 @@
         </is>
       </c>
       <c r="T6" t="n">
-        <v>-1.3</v>
+        <v>1.7</v>
       </c>
       <c r="U6" t="inlineStr"/>
       <c r="V6" t="inlineStr"/>
@@ -1315,59 +1301,57 @@
       </c>
       <c r="X6" t="inlineStr">
         <is>
+          <t>LAL</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="Z6" t="n">
+        <v>38</v>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AD6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AE6" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AF6" t="inlineStr">
+        <is>
+          <t>LAC</t>
+        </is>
+      </c>
+      <c r="AG6" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AH6" t="inlineStr">
+        <is>
           <t>MEM</t>
         </is>
       </c>
-      <c r="Y6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Z6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AA6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AB6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AC6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AD6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AE6" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="AF6" t="inlineStr">
-        <is>
-          <t>SAS</t>
-        </is>
-      </c>
-      <c r="AG6" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AH6" t="inlineStr">
-        <is>
-          <t>DET</t>
-        </is>
-      </c>
       <c r="AI6" t="inlineStr">
         <is>
           <t>vs</t>
@@ -1375,7 +1359,7 @@
       </c>
       <c r="AJ6" t="inlineStr">
         <is>
-          <t>ORL</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="AK6" t="inlineStr">
@@ -1385,45 +1369,45 @@
       </c>
       <c r="AL6" t="inlineStr">
         <is>
-          <t>BKN</t>
+          <t>CHA</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Evan Mobley</t>
+          <t>Jalen Johnson</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>F</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
-        <v>33.4</v>
+        <v>34.6</v>
       </c>
       <c r="G7" t="n">
-        <v>31.8</v>
+        <v>29.9</v>
       </c>
       <c r="H7" t="n">
-        <v>32.3</v>
+        <v>29.2</v>
       </c>
       <c r="I7" t="n">
         <v>6</v>
       </c>
       <c r="J7" t="n">
+        <v>2</v>
+      </c>
+      <c r="K7" t="n">
         <v>1</v>
-      </c>
-      <c r="K7" t="n">
-        <v>2</v>
       </c>
       <c r="L7" t="n">
         <v>1</v>
@@ -1432,19 +1416,23 @@
         <v>2</v>
       </c>
       <c r="N7" t="n">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="O7" t="n">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="P7" t="n">
-        <v>24</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>33</v>
-      </c>
-      <c r="R7" t="n">
-        <v>26</v>
+        <v>12</v>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="S7" t="inlineStr">
         <is>
@@ -1452,7 +1440,7 @@
         </is>
       </c>
       <c r="T7" t="n">
-        <v>1.5</v>
+        <v>-1.8</v>
       </c>
       <c r="U7" t="inlineStr"/>
       <c r="V7" t="inlineStr"/>
@@ -1463,16 +1451,18 @@
       </c>
       <c r="X7" t="inlineStr">
         <is>
-          <t>LAL</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="Y7" t="inlineStr">
         <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="Z7" t="n">
-        <v>38</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="AA7" t="inlineStr">
         <is>
@@ -1496,12 +1486,12 @@
       </c>
       <c r="AE7" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AF7" t="inlineStr">
         <is>
-          <t>LAC</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="AG7" t="inlineStr">
@@ -1511,39 +1501,39 @@
       </c>
       <c r="AH7" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>CHA</t>
         </is>
       </c>
       <c r="AI7" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AJ7" t="inlineStr">
         <is>
+          <t>MIN</t>
+        </is>
+      </c>
+      <c r="AK7" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AL7" t="inlineStr">
+        <is>
           <t>IND</t>
-        </is>
-      </c>
-      <c r="AK7" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AL7" t="inlineStr">
-        <is>
-          <t>CHA</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>DET</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Jaren Jackson Jr.</t>
+          <t>Jalen Duren</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -1558,247 +1548,231 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>28</v>
+        <v>23.6</v>
       </c>
       <c r="G8" t="n">
+        <v>28.2</v>
+      </c>
+      <c r="H8" t="n">
         <v>30.7</v>
       </c>
-      <c r="H8" t="n">
-        <v>30.4</v>
-      </c>
       <c r="I8" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J8" t="n">
+        <v>4</v>
+      </c>
+      <c r="K8" t="n">
         <v>3</v>
       </c>
-      <c r="K8" t="n">
-        <v>2</v>
-      </c>
       <c r="L8" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M8" t="n">
         <v>2</v>
       </c>
       <c r="N8" t="n">
-        <v>66</v>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>14</v>
+      </c>
+      <c r="O8" t="n">
+        <v>1</v>
       </c>
       <c r="P8" t="n">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="Q8" t="n">
-        <v>10</v>
-      </c>
-      <c r="R8" t="n">
-        <v>36</v>
+        <v>27</v>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="T8" t="n">
-        <v>-1.9</v>
+        <v>0.2</v>
       </c>
       <c r="U8" t="n">
-        <v>4.1</v>
+        <v>9.1</v>
       </c>
       <c r="V8" t="n">
         <v>8</v>
       </c>
       <c r="W8" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="X8" t="inlineStr">
         <is>
+          <t>BKN</t>
+        </is>
+      </c>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="Z8" t="n">
+        <v>33</v>
+      </c>
+      <c r="AA8" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AB8" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AD8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AE8" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AF8" t="inlineStr">
+        <is>
           <t>PHI</t>
         </is>
       </c>
-      <c r="Y8" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="Z8" t="n">
-        <v>43</v>
-      </c>
-      <c r="AA8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AB8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AC8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AD8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AE8" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AF8" t="inlineStr">
+      <c r="AG8" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AH8" t="inlineStr">
+        <is>
+          <t>CHI</t>
+        </is>
+      </c>
+      <c r="AI8" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AJ8" t="inlineStr">
+        <is>
+          <t>DAL</t>
+        </is>
+      </c>
+      <c r="AK8" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AL8" t="inlineStr">
         <is>
           <t>SAS</t>
-        </is>
-      </c>
-      <c r="AG8" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="AH8" t="inlineStr">
-        <is>
-          <t>CLE</t>
-        </is>
-      </c>
-      <c r="AI8" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AJ8" t="inlineStr">
-        <is>
-          <t>LAL</t>
-        </is>
-      </c>
-      <c r="AK8" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AL8" t="inlineStr">
-        <is>
-          <t>DEN</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>DET</t>
+          <t>LAL</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Jalen Duren</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Day-To-Day</t>
-        </is>
-      </c>
+          <t>D'Angelo Russell</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>O</t>
-        </is>
-      </c>
+          <t>G</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
-        <v>24</v>
+        <v>21.4</v>
       </c>
       <c r="G9" t="n">
-        <v>29.5</v>
+        <v>27.9</v>
       </c>
       <c r="H9" t="n">
-        <v>31</v>
+        <v>26.2</v>
       </c>
       <c r="I9" t="n">
         <v>12</v>
       </c>
       <c r="J9" t="n">
+        <v>5</v>
+      </c>
+      <c r="K9" t="n">
+        <v>2</v>
+      </c>
+      <c r="L9" t="n">
+        <v>2</v>
+      </c>
+      <c r="M9" t="n">
         <v>3</v>
       </c>
-      <c r="K9" t="n">
-        <v>3</v>
-      </c>
-      <c r="L9" t="n">
-        <v>4</v>
-      </c>
-      <c r="M9" t="n">
+      <c r="N9" t="n">
+        <v>19</v>
+      </c>
+      <c r="O9" t="n">
+        <v>31</v>
+      </c>
+      <c r="P9" t="n">
+        <v>26</v>
+      </c>
+      <c r="Q9" t="n">
         <v>2</v>
       </c>
-      <c r="N9" t="n">
-        <v>1</v>
-      </c>
-      <c r="O9" t="n">
-        <v>50</v>
-      </c>
-      <c r="P9" t="n">
-        <v>27</v>
-      </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="R9" t="n">
+        <v>29</v>
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="T9" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="U9" t="n">
-        <v>8.800000000000001</v>
-      </c>
-      <c r="V9" t="n">
-        <v>8</v>
-      </c>
+        <v>1.7</v>
+      </c>
+      <c r="U9" t="inlineStr"/>
+      <c r="V9" t="inlineStr"/>
       <c r="W9" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="X9" t="inlineStr">
         <is>
-          <t>BKN</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="Y9" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="Z9" t="n">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="AA9" t="inlineStr">
         <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AB9" t="n">
-        <v>33</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="AC9" t="inlineStr">
         <is>
@@ -1812,12 +1786,12 @@
       </c>
       <c r="AE9" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AF9" t="inlineStr">
         <is>
-          <t>PHI</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="AG9" t="inlineStr">
@@ -1827,7 +1801,7 @@
       </c>
       <c r="AH9" t="inlineStr">
         <is>
-          <t>CHI</t>
+          <t>GSW</t>
         </is>
       </c>
       <c r="AI9" t="inlineStr">
@@ -1837,7 +1811,7 @@
       </c>
       <c r="AJ9" t="inlineStr">
         <is>
-          <t>DAL</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="AK9" t="inlineStr">
@@ -1847,7 +1821,7 @@
       </c>
       <c r="AL9" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>NOP</t>
         </is>
       </c>
     </row>
@@ -1870,25 +1844,25 @@
       </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="n">
-        <v>33.6</v>
+        <v>20.6</v>
       </c>
       <c r="G10" t="n">
-        <v>29.1</v>
+        <v>27.5</v>
       </c>
       <c r="H10" t="n">
-        <v>25.9</v>
+        <v>25.6</v>
       </c>
       <c r="I10" t="n">
         <v>13</v>
       </c>
       <c r="J10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K10" t="n">
         <v>7</v>
       </c>
       <c r="L10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M10" t="n">
         <v>3</v>
@@ -1897,24 +1871,24 @@
         <v>22</v>
       </c>
       <c r="O10" t="n">
+        <v>13</v>
+      </c>
+      <c r="P10" t="n">
+        <v>22</v>
+      </c>
+      <c r="Q10" t="n">
         <v>25</v>
       </c>
-      <c r="P10" t="n">
+      <c r="R10" t="n">
         <v>21</v>
       </c>
-      <c r="Q10" t="n">
-        <v>55</v>
-      </c>
-      <c r="R10" t="n">
-        <v>45</v>
-      </c>
       <c r="S10" t="inlineStr">
         <is>
           <t>vs</t>
         </is>
       </c>
       <c r="T10" t="n">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
       <c r="U10" t="inlineStr"/>
       <c r="V10" t="inlineStr"/>
@@ -2000,32 +1974,32 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>BKN</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Michael Porter Jr.</t>
+          <t>Nic Claxton</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>C</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="n">
-        <v>22</v>
+        <v>26.4</v>
       </c>
       <c r="G11" t="n">
-        <v>28.9</v>
+        <v>27.5</v>
       </c>
       <c r="H11" t="n">
-        <v>24.8</v>
+        <v>27.9</v>
       </c>
       <c r="I11" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J11" t="n">
         <v>2</v>
@@ -2037,22 +2011,22 @@
         <v>4</v>
       </c>
       <c r="M11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N11" t="n">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="O11" t="n">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="P11" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Q11" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="R11" t="n">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="S11" t="inlineStr">
         <is>
@@ -2060,7 +2034,7 @@
         </is>
       </c>
       <c r="T11" t="n">
-        <v>1.1</v>
+        <v>-0.2</v>
       </c>
       <c r="U11" t="inlineStr"/>
       <c r="V11" t="inlineStr"/>
@@ -2071,7 +2045,7 @@
       </c>
       <c r="X11" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>DET</t>
         </is>
       </c>
       <c r="Y11" t="inlineStr">
@@ -2080,36 +2054,32 @@
         </is>
       </c>
       <c r="Z11" t="n">
-        <v>-1</v>
+        <v>35</v>
       </c>
       <c r="AA11" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AB11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AB11" t="n">
+        <v>31</v>
       </c>
       <c r="AC11" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AD11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AD11" t="n">
+        <v>24</v>
       </c>
       <c r="AE11" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AF11" t="inlineStr">
         <is>
-          <t>UTA</t>
+          <t>SAC</t>
         </is>
       </c>
       <c r="AG11" t="inlineStr">
@@ -2119,7 +2089,7 @@
       </c>
       <c r="AH11" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>TOR</t>
         </is>
       </c>
       <c r="AI11" t="inlineStr">
@@ -2129,7 +2099,7 @@
       </c>
       <c r="AJ11" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>NYK</t>
         </is>
       </c>
       <c r="AK11" t="inlineStr">
@@ -2139,68 +2109,66 @@
       </c>
       <c r="AL11" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>PHI</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>LAL</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>D'Angelo Russell</t>
+          <t>Michael Porter Jr.</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>F</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="n">
-        <v>23.4</v>
+        <v>22.4</v>
       </c>
       <c r="G12" t="n">
-        <v>28.1</v>
+        <v>26.5</v>
       </c>
       <c r="H12" t="n">
-        <v>26.2</v>
+        <v>24.6</v>
       </c>
       <c r="I12" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J12" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K12" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="L12" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M12" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N12" t="n">
+        <v>11</v>
+      </c>
+      <c r="O12" t="n">
+        <v>28</v>
+      </c>
+      <c r="P12" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q12" t="n">
         <v>26</v>
       </c>
-      <c r="O12" t="n">
-        <v>2</v>
-      </c>
-      <c r="P12" t="n">
-        <v>29</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>47</v>
-      </c>
-      <c r="R12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="R12" t="n">
+        <v>23</v>
       </c>
       <c r="S12" t="inlineStr">
         <is>
@@ -2208,7 +2176,7 @@
         </is>
       </c>
       <c r="T12" t="n">
-        <v>1.7</v>
+        <v>1.4</v>
       </c>
       <c r="U12" t="inlineStr"/>
       <c r="V12" t="inlineStr"/>
@@ -2219,7 +2187,7 @@
       </c>
       <c r="X12" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="Y12" t="inlineStr">
@@ -2228,7 +2196,7 @@
         </is>
       </c>
       <c r="Z12" t="n">
-        <v>12</v>
+        <v>-1</v>
       </c>
       <c r="AA12" t="inlineStr">
         <is>
@@ -2252,24 +2220,24 @@
       </c>
       <c r="AE12" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AF12" t="inlineStr">
         <is>
+          <t>UTA</t>
+        </is>
+      </c>
+      <c r="AG12" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AH12" t="inlineStr">
+        <is>
           <t>MIN</t>
         </is>
       </c>
-      <c r="AG12" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AH12" t="inlineStr">
-        <is>
-          <t>GSW</t>
-        </is>
-      </c>
       <c r="AI12" t="inlineStr">
         <is>
           <t>@</t>
@@ -2277,76 +2245,76 @@
       </c>
       <c r="AJ12" t="inlineStr">
         <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="AK12" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AL12" t="inlineStr">
+        <is>
           <t>MEM</t>
-        </is>
-      </c>
-      <c r="AK12" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="AL12" t="inlineStr">
-        <is>
-          <t>NOP</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>BKN</t>
+          <t>LAL</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Nic Claxton</t>
+          <t>Rui Hachimura</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>F</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="n">
-        <v>25.6</v>
+        <v>34.6</v>
       </c>
       <c r="G13" t="n">
-        <v>28</v>
+        <v>26.4</v>
       </c>
       <c r="H13" t="n">
-        <v>27.8</v>
+        <v>20.1</v>
       </c>
       <c r="I13" t="n">
+        <v>13</v>
+      </c>
+      <c r="J13" t="n">
+        <v>3</v>
+      </c>
+      <c r="K13" t="n">
+        <v>5</v>
+      </c>
+      <c r="L13" t="n">
+        <v>4</v>
+      </c>
+      <c r="M13" t="n">
+        <v>1</v>
+      </c>
+      <c r="N13" t="n">
+        <v>31</v>
+      </c>
+      <c r="O13" t="n">
+        <v>26</v>
+      </c>
+      <c r="P13" t="n">
+        <v>39</v>
+      </c>
+      <c r="Q13" t="n">
         <v>16</v>
       </c>
-      <c r="J13" t="n">
-        <v>2</v>
-      </c>
-      <c r="K13" t="n">
-        <v>7</v>
-      </c>
-      <c r="L13" t="n">
-        <v>5</v>
-      </c>
-      <c r="M13" t="n">
-        <v>2</v>
-      </c>
-      <c r="N13" t="n">
-        <v>17</v>
-      </c>
-      <c r="O13" t="n">
-        <v>21</v>
-      </c>
-      <c r="P13" t="n">
-        <v>21</v>
-      </c>
-      <c r="Q13" t="n">
-        <v>41</v>
-      </c>
       <c r="R13" t="n">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="S13" t="inlineStr">
         <is>
@@ -2354,7 +2322,7 @@
         </is>
       </c>
       <c r="T13" t="n">
-        <v>-0.3</v>
+        <v>-2.7</v>
       </c>
       <c r="U13" t="inlineStr"/>
       <c r="V13" t="inlineStr"/>
@@ -2365,32 +2333,38 @@
       </c>
       <c r="X13" t="inlineStr">
         <is>
-          <t>DET</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="Y13" t="inlineStr">
         <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="Z13" t="n">
-        <v>35</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Z13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="AA13" t="inlineStr">
         <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="AB13" t="n">
-        <v>31</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="AC13" t="inlineStr">
         <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AD13" t="n">
-        <v>24</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AD13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="AE13" t="inlineStr">
         <is>
@@ -2399,7 +2373,7 @@
       </c>
       <c r="AF13" t="inlineStr">
         <is>
-          <t>SAC</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="AG13" t="inlineStr">
@@ -2409,7 +2383,7 @@
       </c>
       <c r="AH13" t="inlineStr">
         <is>
-          <t>TOR</t>
+          <t>GSW</t>
         </is>
       </c>
       <c r="AI13" t="inlineStr">
@@ -2419,7 +2393,7 @@
       </c>
       <c r="AJ13" t="inlineStr">
         <is>
-          <t>NYK</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="AK13" t="inlineStr">
@@ -2429,45 +2403,45 @@
       </c>
       <c r="AL13" t="inlineStr">
         <is>
-          <t>PHI</t>
+          <t>NOP</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>LAL</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Rui Hachimura</t>
+          <t>Bogdan Bogdanovic</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>G</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="n">
-        <v>32</v>
+        <v>32.4</v>
       </c>
       <c r="G14" t="n">
-        <v>25.8</v>
+        <v>25.6</v>
       </c>
       <c r="H14" t="n">
-        <v>19.8</v>
+        <v>21.3</v>
       </c>
       <c r="I14" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J14" t="n">
         <v>4</v>
       </c>
       <c r="K14" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L14" t="n">
         <v>3</v>
@@ -2476,49 +2450,47 @@
         <v>2</v>
       </c>
       <c r="N14" t="n">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="O14" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="P14" t="n">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="Q14" t="n">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="R14" t="n">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="S14" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="T14" t="n">
-        <v>-2.4</v>
+        <v>-2.1</v>
       </c>
       <c r="U14" t="inlineStr"/>
       <c r="V14" t="inlineStr"/>
       <c r="W14" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="X14" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="Y14" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Z14" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="Z14" t="n">
+        <v>56</v>
       </c>
       <c r="AA14" t="inlineStr">
         <is>
@@ -2547,29 +2519,29 @@
       </c>
       <c r="AF14" t="inlineStr">
         <is>
+          <t>MIA</t>
+        </is>
+      </c>
+      <c r="AG14" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AH14" t="inlineStr">
+        <is>
+          <t>CHA</t>
+        </is>
+      </c>
+      <c r="AI14" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AJ14" t="inlineStr">
+        <is>
           <t>MIN</t>
         </is>
       </c>
-      <c r="AG14" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AH14" t="inlineStr">
-        <is>
-          <t>GSW</t>
-        </is>
-      </c>
-      <c r="AI14" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="AJ14" t="inlineStr">
-        <is>
-          <t>MEM</t>
-        </is>
-      </c>
       <c r="AK14" t="inlineStr">
         <is>
           <t>@</t>
@@ -2577,66 +2549,80 @@
       </c>
       <c r="AL14" t="inlineStr">
         <is>
-          <t>NOP</t>
+          <t>IND</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>PHI</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Tobias Harris</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr"/>
+          <t>Trae Young</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>G</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="n">
-        <v>29.2</v>
+        <v>25.4</v>
       </c>
       <c r="G15" t="n">
-        <v>25.7</v>
+        <v>35</v>
       </c>
       <c r="H15" t="n">
-        <v>27.8</v>
+        <v>37.6</v>
       </c>
       <c r="I15" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K15" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L15" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M15" t="n">
-        <v>1</v>
-      </c>
-      <c r="N15" t="n">
-        <v>41</v>
-      </c>
-      <c r="O15" t="n">
-        <v>31</v>
-      </c>
-      <c r="P15" t="n">
-        <v>27</v>
-      </c>
-      <c r="Q15" t="n">
-        <v>13</v>
-      </c>
-      <c r="R15" t="n">
-        <v>34</v>
+        <v>0</v>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="S15" t="inlineStr">
         <is>
@@ -2644,7 +2630,7 @@
         </is>
       </c>
       <c r="T15" t="n">
-        <v>-0.8</v>
+        <v>0.9</v>
       </c>
       <c r="U15" t="inlineStr"/>
       <c r="V15" t="inlineStr"/>
@@ -2655,7 +2641,7 @@
       </c>
       <c r="X15" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="Y15" t="inlineStr">
@@ -2664,7 +2650,7 @@
         </is>
       </c>
       <c r="Z15" t="n">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="AA15" t="inlineStr">
         <is>
@@ -2688,12 +2674,12 @@
       </c>
       <c r="AE15" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AF15" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="AG15" t="inlineStr">
@@ -2703,39 +2689,39 @@
       </c>
       <c r="AH15" t="inlineStr">
         <is>
-          <t>DET</t>
+          <t>CHA</t>
         </is>
       </c>
       <c r="AI15" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AJ15" t="inlineStr">
         <is>
-          <t>ORL</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="AK15" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AL15" t="inlineStr">
         <is>
-          <t>BKN</t>
+          <t>IND</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>DET</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Trae Young</t>
+          <t>Cade Cunningham</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -2748,50 +2734,48 @@
           <t>G</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr"/>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
       <c r="F16" t="n">
-        <v>25.4</v>
+        <v>39.2</v>
       </c>
       <c r="G16" t="n">
-        <v>35</v>
+        <v>33.5</v>
       </c>
       <c r="H16" t="n">
-        <v>37.6</v>
+        <v>32.1</v>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="J16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K16" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L16" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M16" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N16" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="P16" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Q16" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="O16" t="n">
+        <v>59</v>
+      </c>
+      <c r="P16" t="n">
+        <v>44</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>38</v>
       </c>
       <c r="R16" t="inlineStr">
         <is>
@@ -2804,10 +2788,14 @@
         </is>
       </c>
       <c r="T16" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="U16" t="inlineStr"/>
-      <c r="V16" t="inlineStr"/>
+        <v>-1.6</v>
+      </c>
+      <c r="U16" t="n">
+        <v>2</v>
+      </c>
+      <c r="V16" t="n">
+        <v>8</v>
+      </c>
       <c r="W16" t="inlineStr">
         <is>
           <t>@</t>
@@ -2815,75 +2803,383 @@
       </c>
       <c r="X16" t="inlineStr">
         <is>
+          <t>BKN</t>
+        </is>
+      </c>
+      <c r="Y16" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="Z16" t="n">
+        <v>49</v>
+      </c>
+      <c r="AA16" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AB16" t="n">
+        <v>71</v>
+      </c>
+      <c r="AC16" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AD16" t="n">
+        <v>26</v>
+      </c>
+      <c r="AE16" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AF16" t="inlineStr">
+        <is>
+          <t>PHI</t>
+        </is>
+      </c>
+      <c r="AG16" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AH16" t="inlineStr">
+        <is>
+          <t>CHI</t>
+        </is>
+      </c>
+      <c r="AI16" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AJ16" t="inlineStr">
+        <is>
+          <t>DAL</t>
+        </is>
+      </c>
+      <c r="AK16" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AL16" t="inlineStr">
+        <is>
+          <t>SAS</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>MEM</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Jaren Jackson Jr.</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>30.6</v>
+      </c>
+      <c r="G17" t="n">
+        <v>32.5</v>
+      </c>
+      <c r="H17" t="n">
+        <v>30.7</v>
+      </c>
+      <c r="I17" t="n">
+        <v>11</v>
+      </c>
+      <c r="J17" t="n">
+        <v>3</v>
+      </c>
+      <c r="K17" t="n">
+        <v>2</v>
+      </c>
+      <c r="L17" t="n">
+        <v>4</v>
+      </c>
+      <c r="M17" t="n">
+        <v>2</v>
+      </c>
+      <c r="N17" t="n">
+        <v>49</v>
+      </c>
+      <c r="O17" t="n">
+        <v>66</v>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q17" t="n">
+        <v>28</v>
+      </c>
+      <c r="R17" t="n">
+        <v>10</v>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="T17" t="n">
+        <v>-2.2</v>
+      </c>
+      <c r="U17" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="V17" t="n">
+        <v>8</v>
+      </c>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="X17" t="inlineStr">
+        <is>
+          <t>PHI</t>
+        </is>
+      </c>
+      <c r="Y17" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="Z17" t="n">
+        <v>43</v>
+      </c>
+      <c r="AA17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AC17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AD17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AE17" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AF17" t="inlineStr">
+        <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="AG17" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AH17" t="inlineStr">
+        <is>
+          <t>CLE</t>
+        </is>
+      </c>
+      <c r="AI17" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AJ17" t="inlineStr">
+        <is>
+          <t>LAL</t>
+        </is>
+      </c>
+      <c r="AK17" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AL17" t="inlineStr">
+        <is>
           <t>DEN</t>
         </is>
       </c>
-      <c r="Y16" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="Z16" t="n">
-        <v>29</v>
-      </c>
-      <c r="AA16" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AB16" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AC16" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AD16" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AE16" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AF16" t="inlineStr">
-        <is>
-          <t>MIA</t>
-        </is>
-      </c>
-      <c r="AG16" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AH16" t="inlineStr">
-        <is>
-          <t>CHA</t>
-        </is>
-      </c>
-      <c r="AI16" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="AJ16" t="inlineStr">
-        <is>
-          <t>MIN</t>
-        </is>
-      </c>
-      <c r="AK16" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="AL16" t="inlineStr">
-        <is>
-          <t>IND</t>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>PHI</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Tobias Harris</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="n">
+        <v>28</v>
+      </c>
+      <c r="G18" t="n">
+        <v>27.3</v>
+      </c>
+      <c r="H18" t="n">
+        <v>27.8</v>
+      </c>
+      <c r="I18" t="n">
+        <v>11</v>
+      </c>
+      <c r="J18" t="n">
+        <v>3</v>
+      </c>
+      <c r="K18" t="n">
+        <v>4</v>
+      </c>
+      <c r="L18" t="n">
+        <v>3</v>
+      </c>
+      <c r="M18" t="n">
+        <v>1</v>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O18" t="n">
+        <v>28</v>
+      </c>
+      <c r="P18" t="n">
+        <v>41</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>31</v>
+      </c>
+      <c r="R18" t="n">
+        <v>27</v>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="T18" t="n">
+        <v>-0.8</v>
+      </c>
+      <c r="U18" t="inlineStr"/>
+      <c r="V18" t="inlineStr"/>
+      <c r="W18" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="X18" t="inlineStr">
+        <is>
+          <t>MEM</t>
+        </is>
+      </c>
+      <c r="Y18" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="Z18" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AB18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AC18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AD18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AE18" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AF18" t="inlineStr">
+        <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="AG18" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AH18" t="inlineStr">
+        <is>
+          <t>DET</t>
+        </is>
+      </c>
+      <c r="AI18" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AJ18" t="inlineStr">
+        <is>
+          <t>ORL</t>
+        </is>
+      </c>
+      <c r="AK18" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AL18" t="inlineStr">
+        <is>
+          <t>BKN</t>
         </is>
       </c>
     </row>

</xml_diff>